<commit_message>
Week 10 progress 3
Week 10 progress 3
</commit_message>
<xml_diff>
--- a/data/CA_wateruse_2015_v2.xlsx
+++ b/data/CA_wateruse_2015_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hayley\Documents\UW_GISPP\GEOG_575\Lab Activities\unit-3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF08026-7ACC-4397-BCDC-66FEB11F0B2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B63ACFA-46F4-422D-81A1-8FB28DF7CD66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B3B5BB29-DA7B-4A7B-A6F9-87275E83F509}"/>
   </bookViews>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F558E020-3549-454A-9427-54DDB01442CF}">
   <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E6"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,35 +805,35 @@
         <v>91.846287829305453</v>
       </c>
       <c r="S2">
-        <f t="shared" ref="S2:Z17" si="0">(I2/$Q2)*100</f>
+        <f>(I2/$Q2)*100</f>
         <v>0.48987589810581311</v>
       </c>
       <c r="T2">
-        <f t="shared" si="0"/>
+        <f>(J2/$Q2)*100</f>
         <v>2.340518179838885</v>
       </c>
       <c r="U2">
-        <f t="shared" si="0"/>
+        <f>(K2/$Q2)*100</f>
         <v>0.14696276943174394</v>
       </c>
       <c r="V2">
-        <f t="shared" si="0"/>
+        <f>(L2/$Q2)*100</f>
         <v>0</v>
       </c>
       <c r="W2">
-        <f t="shared" si="0"/>
+        <f>(M2/$Q2)*100</f>
         <v>5.1763553233180915</v>
       </c>
       <c r="X2">
-        <f t="shared" si="0"/>
+        <f>(N2/$Q2)*100</f>
         <v>4.1585020683649025</v>
       </c>
       <c r="Y2">
-        <f t="shared" si="0"/>
+        <f>(O2/$Q2)*100</f>
         <v>1.0178532549531896</v>
       </c>
       <c r="Z2">
-        <f t="shared" si="0"/>
+        <f>(P2/$Q2)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -887,43 +887,43 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q59" si="1">SUM(H3,I3,J3,K3,L3,M3,P3)</f>
+        <f>SUM(H3,I3,J3,K3,L3,M3,P3)</f>
         <v>9.8099999999999987</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:W59" si="2">(H3/$Q3)*100</f>
+        <f>(H3/$Q3)*100</f>
         <v>1.0193679918450562</v>
       </c>
       <c r="S3">
-        <f t="shared" si="0"/>
+        <f>(I3/$Q3)*100</f>
         <v>0</v>
       </c>
       <c r="T3">
-        <f t="shared" si="0"/>
+        <f>(J3/$Q3)*100</f>
         <v>0.20387359836901123</v>
       </c>
       <c r="U3">
-        <f t="shared" si="0"/>
+        <f>(K3/$Q3)*100</f>
         <v>0</v>
       </c>
       <c r="V3">
-        <f t="shared" si="0"/>
+        <f>(L3/$Q3)*100</f>
         <v>0</v>
       </c>
       <c r="W3">
-        <f t="shared" si="0"/>
+        <f>(M3/$Q3)*100</f>
         <v>98.776758409785941</v>
       </c>
       <c r="X3">
-        <f t="shared" si="0"/>
+        <f>(N3/$Q3)*100</f>
         <v>98.776758409785941</v>
       </c>
       <c r="Y3">
-        <f t="shared" si="0"/>
+        <f>(O3/$Q3)*100</f>
         <v>0</v>
       </c>
       <c r="Z3">
-        <f t="shared" si="0"/>
+        <f>(P3/$Q3)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -977,43 +977,43 @@
         <v>0.27</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="1"/>
+        <f>SUM(H4,I4,J4,K4,L4,M4,P4)</f>
         <v>39.690000000000005</v>
       </c>
       <c r="R4">
-        <f t="shared" si="2"/>
+        <f>(H4/$Q4)*100</f>
         <v>21.768707482993197</v>
       </c>
       <c r="S4">
-        <f t="shared" si="0"/>
+        <f>(I4/$Q4)*100</f>
         <v>1.0330057949105567</v>
       </c>
       <c r="T4">
-        <f t="shared" si="0"/>
+        <f>(J4/$Q4)*100</f>
         <v>4.913076341647769</v>
       </c>
       <c r="U4">
-        <f t="shared" si="0"/>
+        <f>(K4/$Q4)*100</f>
         <v>0.57949105568153181</v>
       </c>
       <c r="V4">
-        <f t="shared" si="0"/>
+        <f>(L4/$Q4)*100</f>
         <v>18.74527588813303</v>
       </c>
       <c r="W4">
-        <f t="shared" si="0"/>
+        <f>(M4/$Q4)*100</f>
         <v>52.28017132779037</v>
       </c>
       <c r="X4">
-        <f t="shared" si="0"/>
+        <f>(N4/$Q4)*100</f>
         <v>51.549508692365833</v>
       </c>
       <c r="Y4">
-        <f t="shared" si="0"/>
+        <f>(O4/$Q4)*100</f>
         <v>0.73066263542454002</v>
       </c>
       <c r="Z4">
-        <f t="shared" si="0"/>
+        <f>(P4/$Q4)*100</f>
         <v>0.68027210884353739</v>
       </c>
     </row>
@@ -1067,43 +1067,43 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="1"/>
+        <f>SUM(H5,I5,J5,K5,L5,M5,P5)</f>
         <v>808.53</v>
       </c>
       <c r="R5">
-        <f t="shared" si="2"/>
+        <f>(H5/$Q5)*100</f>
         <v>3.5632567746403971</v>
       </c>
       <c r="S5">
-        <f t="shared" si="0"/>
+        <f>(I5/$Q5)*100</f>
         <v>0.49719861971726464</v>
       </c>
       <c r="T5">
-        <f t="shared" si="0"/>
+        <f>(J5/$Q5)*100</f>
         <v>0.18057462308139463</v>
       </c>
       <c r="U5">
-        <f t="shared" si="0"/>
+        <f>(K5/$Q5)*100</f>
         <v>3.5867562118907154E-2</v>
       </c>
       <c r="V5">
-        <f t="shared" si="0"/>
+        <f>(L5/$Q5)*100</f>
         <v>2.6307001595488106</v>
       </c>
       <c r="W5">
-        <f t="shared" si="0"/>
+        <f>(M5/$Q5)*100</f>
         <v>93.092402260893223</v>
       </c>
       <c r="X5">
-        <f t="shared" si="0"/>
+        <f>(N5/$Q5)*100</f>
         <v>93.033035261524006</v>
       </c>
       <c r="Y5">
-        <f t="shared" si="0"/>
+        <f>(O5/$Q5)*100</f>
         <v>5.9366999369225633E-2</v>
       </c>
       <c r="Z5">
-        <f t="shared" si="0"/>
+        <f>(P5/$Q5)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1157,43 +1157,43 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="1"/>
+        <f>SUM(H6,I6,J6,K6,L6,M6,P6)</f>
         <v>15.83</v>
       </c>
       <c r="R6">
-        <f t="shared" si="2"/>
+        <f>(H6/$Q6)*100</f>
         <v>41.629816803537587</v>
       </c>
       <c r="S6">
-        <f t="shared" si="0"/>
+        <f>(I6/$Q6)*100</f>
         <v>1.0739102969046117</v>
       </c>
       <c r="T6">
-        <f t="shared" si="0"/>
+        <f>(J6/$Q6)*100</f>
         <v>0.12634238787113075</v>
       </c>
       <c r="U6">
-        <f t="shared" si="0"/>
+        <f>(K6/$Q6)*100</f>
         <v>1.5792798483891344</v>
       </c>
       <c r="V6">
-        <f t="shared" si="0"/>
+        <f>(L6/$Q6)*100</f>
         <v>0</v>
       </c>
       <c r="W6">
-        <f t="shared" si="0"/>
+        <f>(M6/$Q6)*100</f>
         <v>55.590650663297538</v>
       </c>
       <c r="X6">
-        <f t="shared" si="0"/>
+        <f>(N6/$Q6)*100</f>
         <v>51.674036639292474</v>
       </c>
       <c r="Y6">
-        <f t="shared" si="0"/>
+        <f>(O6/$Q6)*100</f>
         <v>3.9166140240050535</v>
       </c>
       <c r="Z6">
-        <f t="shared" si="0"/>
+        <f>(P6/$Q6)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1247,43 +1247,43 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="1"/>
+        <f>SUM(H7,I7,J7,K7,L7,M7,P7)</f>
         <v>699.06999999999994</v>
       </c>
       <c r="R7">
-        <f t="shared" si="2"/>
+        <f>(H7/$Q7)*100</f>
         <v>0.35189609052026266</v>
       </c>
       <c r="S7">
-        <f t="shared" si="0"/>
+        <f>(I7/$Q7)*100</f>
         <v>0.12015964066545554</v>
       </c>
       <c r="T7">
-        <f t="shared" si="0"/>
+        <f>(J7/$Q7)*100</f>
         <v>0</v>
       </c>
       <c r="U7">
-        <f t="shared" si="0"/>
+        <f>(K7/$Q7)*100</f>
         <v>3.4331325904415864E-2</v>
       </c>
       <c r="V7">
-        <f t="shared" si="0"/>
+        <f>(L7/$Q7)*100</f>
         <v>0</v>
       </c>
       <c r="W7">
-        <f t="shared" si="0"/>
+        <f>(M7/$Q7)*100</f>
         <v>99.453559729354723</v>
       </c>
       <c r="X7">
-        <f t="shared" si="0"/>
+        <f>(N7/$Q7)*100</f>
         <v>99.44354642596592</v>
       </c>
       <c r="Y7">
-        <f t="shared" si="0"/>
+        <f>(O7/$Q7)*100</f>
         <v>1.0013303388787963E-2</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="0"/>
+        <f>(P7/$Q7)*100</f>
         <v>4.0053213555151852E-2</v>
       </c>
     </row>
@@ -1337,7 +1337,7 @@
         <v>18.510000000000002</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="1"/>
+        <f>SUM(H8,I8,J8,K8,L8,M8,P8)</f>
         <v>250.12</v>
       </c>
       <c r="R8">
@@ -1345,35 +1345,35 @@
         <v>55.961138653446341</v>
       </c>
       <c r="S8">
-        <f t="shared" si="0"/>
+        <f>(I8/$Q8)*100</f>
         <v>1.3353590276667198</v>
       </c>
       <c r="T8">
-        <f t="shared" si="0"/>
+        <f>(J8/$Q8)*100</f>
         <v>0.32384455461378542</v>
       </c>
       <c r="U8">
-        <f t="shared" si="0"/>
+        <f>(K8/$Q8)*100</f>
         <v>0.15992323684631377</v>
       </c>
       <c r="V8">
-        <f t="shared" si="0"/>
+        <f>(L8/$Q8)*100</f>
         <v>0</v>
       </c>
       <c r="W8">
-        <f t="shared" si="0"/>
+        <f>(M8/$Q8)*100</f>
         <v>34.819286742363666</v>
       </c>
       <c r="X8">
-        <f t="shared" si="0"/>
+        <f>(N8/$Q8)*100</f>
         <v>33.9437070206301</v>
       </c>
       <c r="Y8">
-        <f t="shared" si="0"/>
+        <f>(O8/$Q8)*100</f>
         <v>0.8755797217335678</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="0"/>
+        <f>(P8/$Q8)*100</f>
         <v>7.4004477850631707</v>
       </c>
     </row>
@@ -1427,43 +1427,43 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="1"/>
+        <f>SUM(H9,I9,J9,K9,L9,M9,P9)</f>
         <v>19.39</v>
       </c>
       <c r="R9">
-        <f t="shared" si="2"/>
+        <f>(H9/$Q9)*100</f>
         <v>12.377514182568333</v>
       </c>
       <c r="S9">
-        <f t="shared" si="0"/>
+        <f>(I9/$Q9)*100</f>
         <v>0</v>
       </c>
       <c r="T9">
-        <f t="shared" si="0"/>
+        <f>(J9/$Q9)*100</f>
         <v>0</v>
       </c>
       <c r="U9">
-        <f t="shared" si="0"/>
+        <f>(K9/$Q9)*100</f>
         <v>2.939659618359979</v>
       </c>
       <c r="V9">
-        <f t="shared" si="0"/>
+        <f>(L9/$Q9)*100</f>
         <v>0</v>
       </c>
       <c r="W9">
-        <f t="shared" si="0"/>
+        <f>(M9/$Q9)*100</f>
         <v>84.682826199071698</v>
       </c>
       <c r="X9">
-        <f t="shared" si="0"/>
+        <f>(N9/$Q9)*100</f>
         <v>84.321815368746783</v>
       </c>
       <c r="Y9">
-        <f t="shared" si="0"/>
+        <f>(O9/$Q9)*100</f>
         <v>0.36101083032490977</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="0"/>
+        <f>(P9/$Q9)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1517,43 +1517,43 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="1"/>
+        <f>SUM(H10,I10,J10,K10,L10,M10,P10)</f>
         <v>55.67</v>
       </c>
       <c r="R10">
-        <f t="shared" si="2"/>
+        <f>(H10/$Q10)*100</f>
         <v>49.937129513202798</v>
       </c>
       <c r="S10">
-        <f t="shared" si="0"/>
+        <f>(I10/$Q10)*100</f>
         <v>1.5987066642716004</v>
       </c>
       <c r="T10">
-        <f t="shared" si="0"/>
+        <f>(J10/$Q10)*100</f>
         <v>3.5925992455541587E-2</v>
       </c>
       <c r="U10">
-        <f t="shared" si="0"/>
+        <f>(K10/$Q10)*100</f>
         <v>0.32333393209987421</v>
       </c>
       <c r="V10">
-        <f t="shared" si="0"/>
+        <f>(L10/$Q10)*100</f>
         <v>0</v>
       </c>
       <c r="W10">
-        <f t="shared" si="0"/>
+        <f>(M10/$Q10)*100</f>
         <v>48.104903897970182</v>
       </c>
       <c r="X10">
-        <f t="shared" si="0"/>
+        <f>(N10/$Q10)*100</f>
         <v>46.057122328004311</v>
       </c>
       <c r="Y10">
-        <f t="shared" si="0"/>
+        <f>(O10/$Q10)*100</f>
         <v>2.0477815699658701</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="0"/>
+        <f>(P10/$Q10)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1607,43 +1607,43 @@
         <v>0.02</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="1"/>
+        <f>SUM(H11,I11,J11,K11,L11,M11,P11)</f>
         <v>1813.6000000000001</v>
       </c>
       <c r="R11">
-        <f t="shared" si="2"/>
+        <f>(H11/$Q11)*100</f>
         <v>8.6612262902514345</v>
       </c>
       <c r="S11">
-        <f t="shared" si="0"/>
+        <f>(I11/$Q11)*100</f>
         <v>0.57951036612262896</v>
       </c>
       <c r="T11">
-        <f t="shared" si="0"/>
+        <f>(J11/$Q11)*100</f>
         <v>0.43449492721658572</v>
       </c>
       <c r="U11">
-        <f t="shared" si="0"/>
+        <f>(K11/$Q11)*100</f>
         <v>0.73003970004411112</v>
       </c>
       <c r="V11">
-        <f t="shared" si="0"/>
+        <f>(L11/$Q11)*100</f>
         <v>0.45434494927216584</v>
       </c>
       <c r="W11">
-        <f t="shared" si="0"/>
+        <f>(M11/$Q11)*100</f>
         <v>89.139280988089979</v>
       </c>
       <c r="X11">
-        <f t="shared" si="0"/>
+        <f>(N11/$Q11)*100</f>
         <v>89.047198941332155</v>
       </c>
       <c r="Y11">
-        <f t="shared" si="0"/>
+        <f>(O11/$Q11)*100</f>
         <v>9.2082046757829716E-2</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="0"/>
+        <f>(P11/$Q11)*100</f>
         <v>1.102779003087781E-3</v>
       </c>
     </row>
@@ -1697,43 +1697,43 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="1"/>
+        <f>SUM(H12,I12,J12,K12,L12,M12,P12)</f>
         <v>665.73</v>
       </c>
       <c r="R12">
-        <f t="shared" si="2"/>
+        <f>(H12/$Q12)*100</f>
         <v>0.38303816862692081</v>
       </c>
       <c r="S12">
-        <f t="shared" si="0"/>
+        <f>(I12/$Q12)*100</f>
         <v>4.0556982560497501E-2</v>
       </c>
       <c r="T12">
-        <f t="shared" si="0"/>
+        <f>(J12/$Q12)*100</f>
         <v>4.2059093025701114E-2</v>
       </c>
       <c r="U12">
-        <f t="shared" si="0"/>
+        <f>(K12/$Q12)*100</f>
         <v>0.29741787211031501</v>
       </c>
       <c r="V12">
-        <f t="shared" si="0"/>
+        <f>(L12/$Q12)*100</f>
         <v>0</v>
       </c>
       <c r="W12">
-        <f t="shared" si="0"/>
+        <f>(M12/$Q12)*100</f>
         <v>99.236927883676557</v>
       </c>
       <c r="X12">
-        <f t="shared" si="0"/>
+        <f>(N12/$Q12)*100</f>
         <v>99.232421552280954</v>
       </c>
       <c r="Y12">
-        <f t="shared" si="0"/>
+        <f>(O12/$Q12)*100</f>
         <v>4.5063313956108329E-3</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="0"/>
+        <f>(P12/$Q12)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1787,43 +1787,43 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="1"/>
+        <f>SUM(H13,I13,J13,K13,L13,M13,P13)</f>
         <v>74.009999999999991</v>
       </c>
       <c r="R13">
-        <f t="shared" si="2"/>
+        <f>(H13/$Q13)*100</f>
         <v>15.52492906364005</v>
       </c>
       <c r="S13">
-        <f t="shared" si="0"/>
+        <f>(I13/$Q13)*100</f>
         <v>0.64856100526955829</v>
       </c>
       <c r="T13">
-        <f t="shared" si="0"/>
+        <f>(J13/$Q13)*100</f>
         <v>0.48642075395216866</v>
       </c>
       <c r="U13">
-        <f t="shared" si="0"/>
+        <f>(K13/$Q13)*100</f>
         <v>2.3104985812728009</v>
       </c>
       <c r="V13">
-        <f t="shared" si="0"/>
+        <f>(L13/$Q13)*100</f>
         <v>0</v>
       </c>
       <c r="W13">
-        <f t="shared" si="0"/>
+        <f>(M13/$Q13)*100</f>
         <v>81.029590595865429</v>
       </c>
       <c r="X13">
-        <f t="shared" si="0"/>
+        <f>(N13/$Q13)*100</f>
         <v>80.50263477908392</v>
       </c>
       <c r="Y13">
-        <f t="shared" si="0"/>
+        <f>(O13/$Q13)*100</f>
         <v>0.52695581678151604</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="0"/>
+        <f>(P13/$Q13)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1877,43 +1877,43 @@
         <v>14.57</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="1"/>
+        <f>SUM(H14,I14,J14,K14,L14,M14,P14)</f>
         <v>1916.6299999999999</v>
       </c>
       <c r="R14">
-        <f t="shared" si="2"/>
+        <f>(H14/$Q14)*100</f>
         <v>1.27672007638407</v>
       </c>
       <c r="S14">
-        <f t="shared" si="0"/>
+        <f>(I14/$Q14)*100</f>
         <v>6.2609893406656472E-2</v>
       </c>
       <c r="T14">
-        <f t="shared" si="0"/>
+        <f>(J14/$Q14)*100</f>
         <v>0.48574842301330989</v>
       </c>
       <c r="U14">
-        <f t="shared" si="0"/>
+        <f>(K14/$Q14)*100</f>
         <v>0.30574497946917251</v>
       </c>
       <c r="V14">
-        <f t="shared" si="0"/>
+        <f>(L14/$Q14)*100</f>
         <v>0.56766303355368541</v>
       </c>
       <c r="W14">
-        <f t="shared" si="0"/>
+        <f>(M14/$Q14)*100</f>
         <v>96.541325138393958</v>
       </c>
       <c r="X14">
-        <f t="shared" si="0"/>
+        <f>(N14/$Q14)*100</f>
         <v>96.517324679254742</v>
       </c>
       <c r="Y14">
-        <f t="shared" si="0"/>
+        <f>(O14/$Q14)*100</f>
         <v>2.4000459139218319E-2</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="0"/>
+        <f>(P14/$Q14)*100</f>
         <v>0.76018845577915406</v>
       </c>
     </row>
@@ -1967,43 +1967,43 @@
         <v>5.68</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="1"/>
+        <f>SUM(H15,I15,J15,K15,L15,M15,P15)</f>
         <v>61.95</v>
       </c>
       <c r="R15">
-        <f t="shared" si="2"/>
+        <f>(H15/$Q15)*100</f>
         <v>3.9063761097659397</v>
       </c>
       <c r="S15">
-        <f t="shared" si="0"/>
+        <f>(I15/$Q15)*100</f>
         <v>0.14527845036319612</v>
       </c>
       <c r="T15">
-        <f t="shared" si="0"/>
+        <f>(J15/$Q15)*100</f>
         <v>1.3397901533494752</v>
       </c>
       <c r="U15">
-        <f t="shared" si="0"/>
+        <f>(K15/$Q15)*100</f>
         <v>0.37126715092816787</v>
       </c>
       <c r="V15">
-        <f t="shared" si="0"/>
+        <f>(L15/$Q15)*100</f>
         <v>56.820016142050044</v>
       </c>
       <c r="W15">
-        <f t="shared" si="0"/>
+        <f>(M15/$Q15)*100</f>
         <v>28.248587570621471</v>
       </c>
       <c r="X15">
-        <f t="shared" si="0"/>
+        <f>(N15/$Q15)*100</f>
         <v>27.71589991928975</v>
       </c>
       <c r="Y15">
-        <f t="shared" si="0"/>
+        <f>(O15/$Q15)*100</f>
         <v>0.53268765133171914</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="0"/>
+        <f>(P15/$Q15)*100</f>
         <v>9.1686844229217108</v>
       </c>
     </row>
@@ -2057,43 +2057,43 @@
         <v>1.03</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="1"/>
+        <f>SUM(H16,I16,J16,K16,L16,M16,P16)</f>
         <v>1915.24</v>
       </c>
       <c r="R16">
-        <f t="shared" si="2"/>
+        <f>(H16/$Q16)*100</f>
         <v>8.8171717382677883</v>
       </c>
       <c r="S16">
-        <f t="shared" si="0"/>
+        <f>(I16/$Q16)*100</f>
         <v>0.12844343267684469</v>
       </c>
       <c r="T16">
-        <f t="shared" si="0"/>
+        <f>(J16/$Q16)*100</f>
         <v>5.6656084877091129</v>
       </c>
       <c r="U16">
-        <f t="shared" si="0"/>
+        <f>(K16/$Q16)*100</f>
         <v>0.63542950230780471</v>
       </c>
       <c r="V16">
-        <f t="shared" si="0"/>
+        <f>(L16/$Q16)*100</f>
         <v>0.23600175434932433</v>
       </c>
       <c r="W16">
-        <f t="shared" si="0"/>
+        <f>(M16/$Q16)*100</f>
         <v>84.463565923852883</v>
       </c>
       <c r="X16">
-        <f t="shared" si="0"/>
+        <f>(N16/$Q16)*100</f>
         <v>84.319980785697879</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="0"/>
+        <f>(O16/$Q16)*100</f>
         <v>0.14358513815500928</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="0"/>
+        <f>(P16/$Q16)*100</f>
         <v>5.3779160836239848E-2</v>
       </c>
     </row>
@@ -2147,43 +2147,43 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="1"/>
+        <f>SUM(H17,I17,J17,K17,L17,M17,P17)</f>
         <v>684.43999999999994</v>
       </c>
       <c r="R17">
-        <f t="shared" si="2"/>
+        <f>(H17/$Q17)*100</f>
         <v>4.2472678394015553</v>
       </c>
       <c r="S17">
-        <f t="shared" si="0"/>
+        <f>(I17/$Q17)*100</f>
         <v>0.4500029220968968</v>
       </c>
       <c r="T17">
-        <f t="shared" si="0"/>
+        <f>(J17/$Q17)*100</f>
         <v>0</v>
       </c>
       <c r="U17">
-        <f t="shared" si="0"/>
+        <f>(K17/$Q17)*100</f>
         <v>2.1725790427210567</v>
       </c>
       <c r="V17">
-        <f t="shared" si="0"/>
+        <f>(L17/$Q17)*100</f>
         <v>0</v>
       </c>
       <c r="W17">
-        <f t="shared" si="0"/>
+        <f>(M17/$Q17)*100</f>
         <v>93.130150195780487</v>
       </c>
       <c r="X17">
-        <f t="shared" si="0"/>
+        <f>(N17/$Q17)*100</f>
         <v>93.087779790777873</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="0"/>
+        <f>(O17/$Q17)*100</f>
         <v>4.2370405002629889E-2</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="0"/>
+        <f>(P17/$Q17)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -2237,43 +2237,43 @@
         <v>4.2</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="1"/>
+        <f>SUM(H18,I18,J18,K18,L18,M18,P18)</f>
         <v>61.17</v>
       </c>
       <c r="R18">
-        <f t="shared" si="2"/>
+        <f>(H18/$Q18)*100</f>
         <v>4.7899297041033186</v>
       </c>
       <c r="S18">
-        <f t="shared" si="2"/>
+        <f>(I18/$Q18)*100</f>
         <v>1.5693967631191759</v>
       </c>
       <c r="T18">
-        <f t="shared" si="2"/>
+        <f>(J18/$Q18)*100</f>
         <v>0.35965342488147783</v>
       </c>
       <c r="U18">
-        <f t="shared" si="2"/>
+        <f>(K18/$Q18)*100</f>
         <v>0.11443518064410658</v>
       </c>
       <c r="V18">
-        <f t="shared" si="2"/>
+        <f>(L18/$Q18)*100</f>
         <v>0</v>
       </c>
       <c r="W18">
-        <f t="shared" si="2"/>
+        <f>(M18/$Q18)*100</f>
         <v>86.300474088605512</v>
       </c>
       <c r="X18">
-        <f t="shared" ref="X18:Z59" si="3">(N18/$Q18)*100</f>
+        <f>(N18/$Q18)*100</f>
         <v>85.842733366029094</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="3"/>
+        <f>(O18/$Q18)*100</f>
         <v>0.45774072257642634</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="3"/>
+        <f>(P18/$Q18)*100</f>
         <v>6.8661108386463958</v>
       </c>
     </row>
@@ -2327,43 +2327,43 @@
         <v>0.38</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="1"/>
+        <f>SUM(H19,I19,J19,K19,L19,M19,P19)</f>
         <v>111.14</v>
       </c>
       <c r="R19">
-        <f t="shared" si="2"/>
+        <f>(H19/$Q19)*100</f>
         <v>3.419111031131906</v>
       </c>
       <c r="S19">
-        <f t="shared" si="2"/>
+        <f>(I19/$Q19)*100</f>
         <v>0</v>
       </c>
       <c r="T19">
-        <f t="shared" si="2"/>
+        <f>(J19/$Q19)*100</f>
         <v>0.30592046068022316</v>
       </c>
       <c r="U19">
-        <f t="shared" si="2"/>
+        <f>(K19/$Q19)*100</f>
         <v>0.58484793953572067</v>
       </c>
       <c r="V19">
-        <f t="shared" si="2"/>
+        <f>(L19/$Q19)*100</f>
         <v>15.556955191650172</v>
       </c>
       <c r="W19">
-        <f t="shared" si="2"/>
+        <f>(M19/$Q19)*100</f>
         <v>79.791254273888796</v>
       </c>
       <c r="X19">
-        <f t="shared" si="3"/>
+        <f>(N19/$Q19)*100</f>
         <v>79.665287025373416</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="3"/>
+        <f>(O19/$Q19)*100</f>
         <v>0.12596724851538602</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="3"/>
+        <f>(P19/$Q19)*100</f>
         <v>0.34191110311319062</v>
       </c>
     </row>
@@ -2417,43 +2417,43 @@
         <v>436</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="1"/>
+        <f>SUM(H20,I20,J20,K20,L20,M20,P20)</f>
         <v>1938.1</v>
       </c>
       <c r="R20">
-        <f t="shared" si="2"/>
+        <f>(H20/$Q20)*100</f>
         <v>64.828440224962605</v>
       </c>
       <c r="S20">
-        <f t="shared" si="2"/>
+        <f>(I20/$Q20)*100</f>
         <v>5.3284144265001805</v>
       </c>
       <c r="T20">
-        <f t="shared" si="2"/>
+        <f>(J20/$Q20)*100</f>
         <v>5.5404777875238631</v>
       </c>
       <c r="U20">
-        <f t="shared" si="2"/>
+        <f>(K20/$Q20)*100</f>
         <v>1.9090862184613797E-2</v>
       </c>
       <c r="V20">
-        <f t="shared" si="2"/>
+        <f>(L20/$Q20)*100</f>
         <v>2.0638769929312217E-3</v>
       </c>
       <c r="W20">
-        <f t="shared" si="2"/>
+        <f>(M20/$Q20)*100</f>
         <v>1.7852535988855067</v>
       </c>
       <c r="X20">
-        <f t="shared" si="3"/>
+        <f>(N20/$Q20)*100</f>
         <v>0.90965378463443569</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="3"/>
+        <f>(O20/$Q20)*100</f>
         <v>0.87559981425107059</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="3"/>
+        <f>(P20/$Q20)*100</f>
         <v>22.496259222950314</v>
       </c>
     </row>
@@ -2507,43 +2507,43 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="1"/>
+        <f>SUM(H21,I21,J21,K21,L21,M21,P21)</f>
         <v>798.81999999999994</v>
       </c>
       <c r="R21">
-        <f t="shared" si="2"/>
+        <f>(H21/$Q21)*100</f>
         <v>1.9566360381562806</v>
       </c>
       <c r="S21">
-        <f t="shared" si="2"/>
+        <f>(I21/$Q21)*100</f>
         <v>0.57209383841165729</v>
       </c>
       <c r="T21">
-        <f t="shared" si="2"/>
+        <f>(J21/$Q21)*100</f>
         <v>1.2518464735484841E-3</v>
       </c>
       <c r="U21">
-        <f t="shared" si="2"/>
+        <f>(K21/$Q21)*100</f>
         <v>0.77364112065296309</v>
       </c>
       <c r="V21">
-        <f t="shared" si="2"/>
+        <f>(L21/$Q21)*100</f>
         <v>0</v>
       </c>
       <c r="W21">
-        <f t="shared" si="2"/>
+        <f>(M21/$Q21)*100</f>
         <v>96.696377156305559</v>
       </c>
       <c r="X21">
-        <f t="shared" si="3"/>
+        <f>(N21/$Q21)*100</f>
         <v>96.589970206053948</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="3"/>
+        <f>(O21/$Q21)*100</f>
         <v>0.10640695025162115</v>
       </c>
       <c r="Z21">
-        <f t="shared" si="3"/>
+        <f>(P21/$Q21)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -2597,43 +2597,43 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="1"/>
+        <f>SUM(H22,I22,J22,K22,L22,M22,P22)</f>
         <v>70.63000000000001</v>
       </c>
       <c r="R22">
-        <f t="shared" si="2"/>
+        <f>(H22/$Q22)*100</f>
         <v>39.912218603992635</v>
       </c>
       <c r="S22">
-        <f t="shared" si="2"/>
+        <f>(I22/$Q22)*100</f>
         <v>0.28316579357213645</v>
       </c>
       <c r="T22">
-        <f t="shared" si="2"/>
+        <f>(J22/$Q22)*100</f>
         <v>4.2474869035820463E-2</v>
       </c>
       <c r="U22">
-        <f t="shared" si="2"/>
+        <f>(K22/$Q22)*100</f>
         <v>1.6848364717542117</v>
       </c>
       <c r="V22">
-        <f t="shared" si="2"/>
+        <f>(L22/$Q22)*100</f>
         <v>0</v>
       </c>
       <c r="W22">
-        <f t="shared" si="2"/>
+        <f>(M22/$Q22)*100</f>
         <v>58.077304261645189</v>
       </c>
       <c r="X22">
-        <f t="shared" si="3"/>
+        <f>(N22/$Q22)*100</f>
         <v>57.341073198357627</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="3"/>
+        <f>(O22/$Q22)*100</f>
         <v>0.73623106328755472</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="3"/>
+        <f>(P22/$Q22)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -2687,43 +2687,43 @@
         <v>0</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="1"/>
+        <f>SUM(H23,I23,J23,K23,L23,M23,P23)</f>
         <v>18.57</v>
       </c>
       <c r="R23">
-        <f t="shared" si="2"/>
+        <f>(H23/$Q23)*100</f>
         <v>3.6618201400107702</v>
       </c>
       <c r="S23">
-        <f t="shared" si="2"/>
+        <f>(I23/$Q23)*100</f>
         <v>0</v>
       </c>
       <c r="T23">
-        <f t="shared" si="2"/>
+        <f>(J23/$Q23)*100</f>
         <v>0.26925148088314488</v>
       </c>
       <c r="U23">
-        <f t="shared" si="2"/>
+        <f>(K23/$Q23)*100</f>
         <v>2.1001615508885298</v>
       </c>
       <c r="V23">
-        <f t="shared" si="2"/>
+        <f>(L23/$Q23)*100</f>
         <v>0</v>
       </c>
       <c r="W23">
-        <f t="shared" si="2"/>
+        <f>(M23/$Q23)*100</f>
         <v>93.968766828217554</v>
       </c>
       <c r="X23">
-        <f t="shared" si="3"/>
+        <f>(N23/$Q23)*100</f>
         <v>93.753365643511046</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="3"/>
+        <f>(O23/$Q23)*100</f>
         <v>0.2154011847065159</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="3"/>
+        <f>(P23/$Q23)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -2777,43 +2777,43 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="1"/>
+        <f>SUM(H24,I24,J24,K24,L24,M24,P24)</f>
         <v>81.41</v>
       </c>
       <c r="R24">
-        <f t="shared" si="2"/>
+        <f>(H24/$Q24)*100</f>
         <v>10.846333374278345</v>
       </c>
       <c r="S24">
-        <f t="shared" si="2"/>
+        <f>(I24/$Q24)*100</f>
         <v>4.1149735904680016</v>
       </c>
       <c r="T24">
-        <f t="shared" si="2"/>
+        <f>(J24/$Q24)*100</f>
         <v>0.20881955533718222</v>
       </c>
       <c r="U24">
-        <f t="shared" si="2"/>
+        <f>(K24/$Q24)*100</f>
         <v>0.42992261392949271</v>
       </c>
       <c r="V24">
-        <f t="shared" si="2"/>
+        <f>(L24/$Q24)*100</f>
         <v>1.2283503255128362E-2</v>
       </c>
       <c r="W24">
-        <f t="shared" si="2"/>
+        <f>(M24/$Q24)*100</f>
         <v>84.387667362731861</v>
       </c>
       <c r="X24">
-        <f t="shared" si="3"/>
+        <f>(N24/$Q24)*100</f>
         <v>84.215698317160061</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="3"/>
+        <f>(O24/$Q24)*100</f>
         <v>0.1719690455717971</v>
       </c>
       <c r="Z24">
-        <f t="shared" si="3"/>
+        <f>(P24/$Q24)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -2871,39 +2871,39 @@
         <v>1086.56</v>
       </c>
       <c r="R25">
-        <f t="shared" si="2"/>
+        <f>(H25/$Q25)*100</f>
         <v>4.6173243999410989</v>
       </c>
       <c r="S25">
-        <f t="shared" si="2"/>
+        <f>(I25/$Q25)*100</f>
         <v>0.51814902076277425</v>
       </c>
       <c r="T25">
-        <f t="shared" si="2"/>
+        <f>(J25/$Q25)*100</f>
         <v>6.8104844647327342E-2</v>
       </c>
       <c r="U25">
-        <f t="shared" si="2"/>
+        <f>(K25/$Q25)*100</f>
         <v>2.2879546458548079</v>
       </c>
       <c r="V25">
-        <f t="shared" si="2"/>
+        <f>(L25/$Q25)*100</f>
         <v>3.1595125901929024</v>
       </c>
       <c r="W25">
-        <f t="shared" si="2"/>
+        <f>(M25/$Q25)*100</f>
         <v>89.329627448093078</v>
       </c>
       <c r="X25">
-        <f t="shared" si="3"/>
+        <f>(N25/$Q25)*100</f>
         <v>89.305698718892657</v>
       </c>
       <c r="Y25">
-        <f t="shared" si="3"/>
+        <f>(O25/$Q25)*100</f>
         <v>2.3928729200412311E-2</v>
       </c>
       <c r="Z25">
-        <f t="shared" si="3"/>
+        <f>(P25/$Q25)*100</f>
         <v>1.9327050508025329E-2</v>
       </c>
     </row>
@@ -2957,43 +2957,43 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="1"/>
+        <f>SUM(H26,I26,J26,K26,L26,M26,P26)</f>
         <v>173.26000000000002</v>
       </c>
       <c r="R26">
-        <f t="shared" si="2"/>
+        <f>(H26/$Q26)*100</f>
         <v>0.34630035784370305</v>
       </c>
       <c r="S26">
-        <f t="shared" si="2"/>
+        <f>(I26/$Q26)*100</f>
         <v>0</v>
       </c>
       <c r="T26">
-        <f t="shared" si="2"/>
+        <f>(J26/$Q26)*100</f>
         <v>4.6173381045827078E-2</v>
       </c>
       <c r="U26">
-        <f t="shared" si="2"/>
+        <f>(K26/$Q26)*100</f>
         <v>0.47327715571972745</v>
       </c>
       <c r="V26">
-        <f t="shared" si="2"/>
+        <f>(L26/$Q26)*100</f>
         <v>0.15583516102966638</v>
       </c>
       <c r="W26">
-        <f t="shared" si="2"/>
+        <f>(M26/$Q26)*100</f>
         <v>98.978413944361066</v>
       </c>
       <c r="X26">
-        <f t="shared" si="3"/>
+        <f>(N26/$Q26)*100</f>
         <v>98.787948747547034</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="3"/>
+        <f>(O26/$Q26)*100</f>
         <v>0.1904651968140367</v>
       </c>
       <c r="Z26">
-        <f t="shared" si="3"/>
+        <f>(P26/$Q26)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -3047,43 +3047,43 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="1"/>
+        <f>SUM(H27,I27,J27,K27,L27,M27,P27)</f>
         <v>70.8</v>
       </c>
       <c r="R27">
-        <f t="shared" si="2"/>
+        <f>(H27/$Q27)*100</f>
         <v>2.7966101694915255</v>
       </c>
       <c r="S27">
-        <f t="shared" si="2"/>
+        <f>(I27/$Q27)*100</f>
         <v>4.2372881355932202E-2</v>
       </c>
       <c r="T27">
-        <f t="shared" si="2"/>
+        <f>(J27/$Q27)*100</f>
         <v>2.8248587570621469E-2</v>
       </c>
       <c r="U27">
-        <f t="shared" si="2"/>
+        <f>(K27/$Q27)*100</f>
         <v>9.887005649717516E-2</v>
       </c>
       <c r="V27">
-        <f t="shared" si="2"/>
+        <f>(L27/$Q27)*100</f>
         <v>14.364406779661017</v>
       </c>
       <c r="W27">
-        <f t="shared" si="2"/>
+        <f>(M27/$Q27)*100</f>
         <v>82.669491525423737</v>
       </c>
       <c r="X27">
-        <f t="shared" si="3"/>
+        <f>(N27/$Q27)*100</f>
         <v>82.401129943502838</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="3"/>
+        <f>(O27/$Q27)*100</f>
         <v>0.26836158192090398</v>
       </c>
       <c r="Z27">
-        <f t="shared" si="3"/>
+        <f>(P27/$Q27)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -3137,43 +3137,43 @@
         <v>160.66</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="1"/>
+        <f>SUM(H28,I28,J28,K28,L28,M28,P28)</f>
         <v>377.49</v>
       </c>
       <c r="R28">
-        <f t="shared" si="2"/>
+        <f>(H28/$Q28)*100</f>
         <v>10.127420593923016</v>
       </c>
       <c r="S28">
-        <f t="shared" si="2"/>
+        <f>(I28/$Q28)*100</f>
         <v>0.57220058809504892</v>
       </c>
       <c r="T28">
-        <f t="shared" si="2"/>
+        <f>(J28/$Q28)*100</f>
         <v>1.7510397626427192</v>
       </c>
       <c r="U28">
-        <f t="shared" si="2"/>
+        <f>(K28/$Q28)*100</f>
         <v>0.25696044928342471</v>
       </c>
       <c r="V28">
-        <f t="shared" si="2"/>
+        <f>(L28/$Q28)*100</f>
         <v>0</v>
       </c>
       <c r="W28">
-        <f t="shared" si="2"/>
+        <f>(M28/$Q28)*100</f>
         <v>44.732310789689791</v>
       </c>
       <c r="X28">
-        <f t="shared" si="3"/>
+        <f>(N28/$Q28)*100</f>
         <v>44.205144507139259</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="3"/>
+        <f>(O28/$Q28)*100</f>
         <v>0.52716628255053111</v>
       </c>
       <c r="Z28">
-        <f t="shared" si="3"/>
+        <f>(P28/$Q28)*100</f>
         <v>42.560067816365994</v>
       </c>
     </row>
@@ -3227,43 +3227,43 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="1"/>
+        <f>SUM(H29,I29,J29,K29,L29,M29,P29)</f>
         <v>126.28</v>
       </c>
       <c r="R29">
-        <f t="shared" si="2"/>
+        <f>(H29/$Q29)*100</f>
         <v>12.100095026924294</v>
       </c>
       <c r="S29">
-        <f t="shared" si="2"/>
+        <f>(I29/$Q29)*100</f>
         <v>5.9787773202407353</v>
       </c>
       <c r="T29">
-        <f t="shared" si="2"/>
+        <f>(J29/$Q29)*100</f>
         <v>0</v>
       </c>
       <c r="U29">
-        <f t="shared" si="2"/>
+        <f>(K29/$Q29)*100</f>
         <v>0.12670256572695598</v>
       </c>
       <c r="V29">
-        <f t="shared" si="2"/>
+        <f>(L29/$Q29)*100</f>
         <v>0.46721571111815013</v>
       </c>
       <c r="W29">
-        <f t="shared" si="2"/>
+        <f>(M29/$Q29)*100</f>
         <v>81.327209375989867</v>
       </c>
       <c r="X29">
-        <f t="shared" si="3"/>
+        <f>(N29/$Q29)*100</f>
         <v>80.725372188786821</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="3"/>
+        <f>(O29/$Q29)*100</f>
         <v>0.60183718720304091</v>
       </c>
       <c r="Z29">
-        <f t="shared" si="3"/>
+        <f>(P29/$Q29)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -3317,43 +3317,43 @@
         <v>0</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="1"/>
+        <f>SUM(H30,I30,J30,K30,L30,M30,P30)</f>
         <v>60.449999999999996</v>
       </c>
       <c r="R30">
-        <f t="shared" si="2"/>
+        <f>(H30/$Q30)*100</f>
         <v>18.9247311827957</v>
       </c>
       <c r="S30">
-        <f t="shared" si="2"/>
+        <f>(I30/$Q30)*100</f>
         <v>0.13234077750206785</v>
       </c>
       <c r="T30">
-        <f t="shared" si="2"/>
+        <f>(J30/$Q30)*100</f>
         <v>0.62861869313482222</v>
       </c>
       <c r="U30">
-        <f t="shared" si="2"/>
+        <f>(K30/$Q30)*100</f>
         <v>0.18196856906534328</v>
       </c>
       <c r="V30">
-        <f t="shared" si="2"/>
+        <f>(L30/$Q30)*100</f>
         <v>0</v>
       </c>
       <c r="W30">
-        <f t="shared" si="2"/>
+        <f>(M30/$Q30)*100</f>
         <v>80.132340777502066</v>
       </c>
       <c r="X30">
-        <f t="shared" si="3"/>
+        <f>(N30/$Q30)*100</f>
         <v>78.081058726220036</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="3"/>
+        <f>(O30/$Q30)*100</f>
         <v>2.0512820512820511</v>
       </c>
       <c r="Z30">
-        <f t="shared" si="3"/>
+        <f>(P30/$Q30)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -3407,43 +3407,43 @@
         <v>62.36</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="1"/>
+        <f>SUM(H31,I31,J31,K31,L31,M31,P31)</f>
         <v>561.79</v>
       </c>
       <c r="R31">
-        <f t="shared" si="2"/>
+        <f>(H31/$Q31)*100</f>
         <v>81.443243916766065</v>
       </c>
       <c r="S31">
-        <f t="shared" si="2"/>
+        <f>(I31/$Q31)*100</f>
         <v>3.2236244860179073</v>
       </c>
       <c r="T31">
-        <f t="shared" si="2"/>
+        <f>(J31/$Q31)*100</f>
         <v>2.1111091333060399</v>
       </c>
       <c r="U31">
-        <f t="shared" si="2"/>
+        <f>(K31/$Q31)*100</f>
         <v>5.3400736930169631E-3</v>
       </c>
       <c r="V31">
-        <f t="shared" si="2"/>
+        <f>(L31/$Q31)*100</f>
         <v>0</v>
       </c>
       <c r="W31">
-        <f t="shared" si="2"/>
+        <f>(M31/$Q31)*100</f>
         <v>2.1164492069990568</v>
       </c>
       <c r="X31">
-        <f t="shared" si="3"/>
+        <f>(N31/$Q31)*100</f>
         <v>0.452126239342103</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="3"/>
+        <f>(O31/$Q31)*100</f>
         <v>1.6643229676569535</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="3"/>
+        <f>(P31/$Q31)*100</f>
         <v>11.100233183217929</v>
       </c>
     </row>
@@ -3497,43 +3497,43 @@
         <v>0</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="1"/>
+        <f>SUM(H32,I32,J32,K32,L32,M32,P32)</f>
         <v>190.07</v>
       </c>
       <c r="R32">
-        <f t="shared" si="2"/>
+        <f>(H32/$Q32)*100</f>
         <v>28.447414110590834</v>
       </c>
       <c r="S32">
-        <f t="shared" si="2"/>
+        <f>(I32/$Q32)*100</f>
         <v>1.0101541537328351</v>
       </c>
       <c r="T32">
-        <f t="shared" si="2"/>
+        <f>(J32/$Q32)*100</f>
         <v>0.15783658652075552</v>
       </c>
       <c r="U32">
-        <f t="shared" si="2"/>
+        <f>(K32/$Q32)*100</f>
         <v>0.15783658652075552</v>
       </c>
       <c r="V32">
-        <f t="shared" si="2"/>
+        <f>(L32/$Q32)*100</f>
         <v>0</v>
       </c>
       <c r="W32">
-        <f t="shared" si="2"/>
+        <f>(M32/$Q32)*100</f>
         <v>70.226758562634814</v>
       </c>
       <c r="X32">
-        <f t="shared" si="3"/>
+        <f>(N32/$Q32)*100</f>
         <v>68.532645867312041</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="3"/>
+        <f>(O32/$Q32)*100</f>
         <v>1.6941126953227761</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="3"/>
+        <f>(P32/$Q32)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -3587,43 +3587,43 @@
         <v>0</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="1"/>
+        <f>SUM(H33,I33,J33,K33,L33,M33,P33)</f>
         <v>106.86</v>
       </c>
       <c r="R33">
-        <f t="shared" si="2"/>
+        <f>(H33/$Q33)*100</f>
         <v>2.011978289350552</v>
       </c>
       <c r="S33">
-        <f t="shared" si="2"/>
+        <f>(I33/$Q33)*100</f>
         <v>1.2633352049410445</v>
       </c>
       <c r="T33">
-        <f t="shared" si="2"/>
+        <f>(J33/$Q33)*100</f>
         <v>0.27138311809844656</v>
       </c>
       <c r="U33">
-        <f t="shared" si="2"/>
+        <f>(K33/$Q33)*100</f>
         <v>0.25266704098820886</v>
       </c>
       <c r="V33">
-        <f t="shared" si="2"/>
+        <f>(L33/$Q33)*100</f>
         <v>1.8716077110237695E-2</v>
       </c>
       <c r="W33">
-        <f t="shared" si="2"/>
+        <f>(M33/$Q33)*100</f>
         <v>96.181920269511508</v>
       </c>
       <c r="X33">
-        <f t="shared" si="3"/>
+        <f>(N33/$Q33)*100</f>
         <v>95.171252105558679</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="3"/>
+        <f>(O33/$Q33)*100</f>
         <v>1.0106681639528354</v>
       </c>
       <c r="Z33">
-        <f t="shared" si="3"/>
+        <f>(P33/$Q33)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -3677,43 +3677,43 @@
         <v>1.46</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="1"/>
+        <f>SUM(H34,I34,J34,K34,L34,M34,P34)</f>
         <v>1222.47</v>
       </c>
       <c r="R34">
-        <f t="shared" si="2"/>
+        <f>(H34/$Q34)*100</f>
         <v>36.052418464256789</v>
       </c>
       <c r="S34">
-        <f t="shared" si="2"/>
+        <f>(I34/$Q34)*100</f>
         <v>0.42782235964890752</v>
       </c>
       <c r="T34">
-        <f t="shared" si="2"/>
+        <f>(J34/$Q34)*100</f>
         <v>0.93581028573298319</v>
       </c>
       <c r="U34">
-        <f t="shared" si="2"/>
+        <f>(K34/$Q34)*100</f>
         <v>0.33947663337341616</v>
       </c>
       <c r="V34">
-        <f t="shared" si="2"/>
+        <f>(L34/$Q34)*100</f>
         <v>1.4454342437851238</v>
       </c>
       <c r="W34">
-        <f t="shared" si="2"/>
+        <f>(M34/$Q34)*100</f>
         <v>60.679607679534051</v>
       </c>
       <c r="X34">
-        <f t="shared" si="3"/>
+        <f>(N34/$Q34)*100</f>
         <v>58.280366798367247</v>
       </c>
       <c r="Y34">
-        <f t="shared" si="3"/>
+        <f>(O34/$Q34)*100</f>
         <v>2.3992408811668176</v>
       </c>
       <c r="Z34">
-        <f t="shared" si="3"/>
+        <f>(P34/$Q34)*100</f>
         <v>0.11943033366871988</v>
       </c>
     </row>
@@ -3767,43 +3767,43 @@
         <v>1.89</v>
       </c>
       <c r="Q35">
-        <f t="shared" si="1"/>
+        <f>SUM(H35,I35,J35,K35,L35,M35,P35)</f>
         <v>867.58</v>
       </c>
       <c r="R35">
-        <f t="shared" si="2"/>
+        <f>(H35/$Q35)*100</f>
         <v>26.659212983240739</v>
       </c>
       <c r="S35">
-        <f t="shared" si="2"/>
+        <f>(I35/$Q35)*100</f>
         <v>1.9490997948316005</v>
       </c>
       <c r="T35">
-        <f t="shared" si="2"/>
+        <f>(J35/$Q35)*100</f>
         <v>0.25127365776066762</v>
       </c>
       <c r="U35">
-        <f t="shared" si="2"/>
+        <f>(K35/$Q35)*100</f>
         <v>0.20977892528642891</v>
       </c>
       <c r="V35">
-        <f t="shared" si="2"/>
+        <f>(L35/$Q35)*100</f>
         <v>19.759561077940941</v>
       </c>
       <c r="W35">
-        <f t="shared" si="2"/>
+        <f>(M35/$Q35)*100</f>
         <v>50.953226215449867</v>
       </c>
       <c r="X35">
-        <f t="shared" si="3"/>
+        <f>(N35/$Q35)*100</f>
         <v>50.758431499112476</v>
       </c>
       <c r="Y35">
-        <f t="shared" si="3"/>
+        <f>(O35/$Q35)*100</f>
         <v>0.19479471633739828</v>
       </c>
       <c r="Z35">
-        <f t="shared" si="3"/>
+        <f>(P35/$Q35)*100</f>
         <v>0.2178473454897531</v>
       </c>
     </row>
@@ -3857,43 +3857,43 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="1"/>
+        <f>SUM(H36,I36,J36,K36,L36,M36,P36)</f>
         <v>25.299999999999997</v>
       </c>
       <c r="R36">
-        <f t="shared" si="2"/>
+        <f>(H36/$Q36)*100</f>
         <v>20.711462450592887</v>
       </c>
       <c r="S36">
-        <f t="shared" si="2"/>
+        <f>(I36/$Q36)*100</f>
         <v>15.889328063241107</v>
       </c>
       <c r="T36">
-        <f t="shared" si="2"/>
+        <f>(J36/$Q36)*100</f>
         <v>1.1067193675889331</v>
       </c>
       <c r="U36">
-        <f t="shared" si="2"/>
+        <f>(K36/$Q36)*100</f>
         <v>2.5296442687747041</v>
       </c>
       <c r="V36">
-        <f t="shared" si="2"/>
+        <f>(L36/$Q36)*100</f>
         <v>0</v>
       </c>
       <c r="W36">
-        <f t="shared" si="2"/>
+        <f>(M36/$Q36)*100</f>
         <v>59.762845849802368</v>
       </c>
       <c r="X36">
-        <f t="shared" si="3"/>
+        <f>(N36/$Q36)*100</f>
         <v>58.735177865612656</v>
       </c>
       <c r="Y36">
-        <f t="shared" si="3"/>
+        <f>(O36/$Q36)*100</f>
         <v>1.0276679841897234</v>
       </c>
       <c r="Z36">
-        <f t="shared" si="3"/>
+        <f>(P36/$Q36)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -3947,43 +3947,43 @@
         <v>13.04</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="1"/>
+        <f>SUM(H37,I37,J37,K37,L37,M37,P37)</f>
         <v>457.3</v>
       </c>
       <c r="R37">
-        <f t="shared" si="2"/>
+        <f>(H37/$Q37)*100</f>
         <v>73.84649026897003</v>
       </c>
       <c r="S37">
-        <f t="shared" si="2"/>
+        <f>(I37/$Q37)*100</f>
         <v>10.061228952547561</v>
       </c>
       <c r="T37">
-        <f t="shared" si="2"/>
+        <f>(J37/$Q37)*100</f>
         <v>2.1823748086595236</v>
       </c>
       <c r="U37">
-        <f t="shared" si="2"/>
+        <f>(K37/$Q37)*100</f>
         <v>1.5001093374152636</v>
       </c>
       <c r="V37">
-        <f t="shared" si="2"/>
+        <f>(L37/$Q37)*100</f>
         <v>2.2698447408703259</v>
       </c>
       <c r="W37">
-        <f t="shared" si="2"/>
+        <f>(M37/$Q37)*100</f>
         <v>7.288432101465121</v>
       </c>
       <c r="X37">
-        <f t="shared" si="3"/>
+        <f>(N37/$Q37)*100</f>
         <v>6.0835337852613165</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="3"/>
+        <f>(O37/$Q37)*100</f>
         <v>1.2048983162038049</v>
       </c>
       <c r="Z37">
-        <f t="shared" si="3"/>
+        <f>(P37/$Q37)*100</f>
         <v>2.8515197900721625</v>
       </c>
     </row>
@@ -4037,43 +4037,43 @@
         <v>80.58</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="1"/>
+        <f>SUM(H38,I38,J38,K38,L38,M38,P38)</f>
         <v>613.33000000000004</v>
       </c>
       <c r="R38">
-        <f t="shared" si="2"/>
+        <f>(H38/$Q38)*100</f>
         <v>66.655797042375227</v>
       </c>
       <c r="S38">
-        <f t="shared" si="2"/>
+        <f>(I38/$Q38)*100</f>
         <v>0.26413187028190371</v>
       </c>
       <c r="T38">
-        <f t="shared" si="2"/>
+        <f>(J38/$Q38)*100</f>
         <v>0.48424176218349013</v>
       </c>
       <c r="U38">
-        <f t="shared" si="2"/>
+        <f>(K38/$Q38)*100</f>
         <v>0.17282702623383822</v>
       </c>
       <c r="V38">
-        <f t="shared" si="2"/>
+        <f>(L38/$Q38)*100</f>
         <v>0</v>
       </c>
       <c r="W38">
-        <f t="shared" si="2"/>
+        <f>(M38/$Q38)*100</f>
         <v>19.2848874178664</v>
       </c>
       <c r="X38">
-        <f t="shared" si="3"/>
+        <f>(N38/$Q38)*100</f>
         <v>16.674547144277955</v>
       </c>
       <c r="Y38">
-        <f t="shared" si="3"/>
+        <f>(O38/$Q38)*100</f>
         <v>2.6103402735884433</v>
       </c>
       <c r="Z38">
-        <f t="shared" si="3"/>
+        <f>(P38/$Q38)*100</f>
         <v>13.138114881059135</v>
       </c>
     </row>
@@ -4127,43 +4127,43 @@
         <v>0</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="1"/>
+        <f>SUM(H39,I39,J39,K39,L39,M39,P39)</f>
         <v>68.2</v>
       </c>
       <c r="R39">
-        <f t="shared" si="2"/>
+        <f>(H39/$Q39)*100</f>
         <v>99.032258064516128</v>
       </c>
       <c r="S39">
-        <f t="shared" si="2"/>
+        <f>(I39/$Q39)*100</f>
         <v>0</v>
       </c>
       <c r="T39">
-        <f t="shared" si="2"/>
+        <f>(J39/$Q39)*100</f>
         <v>0.11730205278592376</v>
       </c>
       <c r="U39">
-        <f t="shared" si="2"/>
+        <f>(K39/$Q39)*100</f>
         <v>0</v>
       </c>
       <c r="V39">
-        <f t="shared" si="2"/>
+        <f>(L39/$Q39)*100</f>
         <v>0</v>
       </c>
       <c r="W39">
-        <f t="shared" si="2"/>
+        <f>(M39/$Q39)*100</f>
         <v>0.85043988269794712</v>
       </c>
       <c r="X39">
-        <f t="shared" si="3"/>
+        <f>(N39/$Q39)*100</f>
         <v>0</v>
       </c>
       <c r="Y39">
-        <f t="shared" si="3"/>
+        <f>(O39/$Q39)*100</f>
         <v>0.85043988269794712</v>
       </c>
       <c r="Z39">
-        <f t="shared" si="3"/>
+        <f>(P39/$Q39)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -4217,43 +4217,43 @@
         <v>0</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="1"/>
+        <f>SUM(H40,I40,J40,K40,L40,M40,P40)</f>
         <v>1329.75</v>
       </c>
       <c r="R40">
-        <f t="shared" si="2"/>
+        <f>(H40/$Q40)*100</f>
         <v>7.0231246474901292</v>
       </c>
       <c r="S40">
-        <f t="shared" si="2"/>
+        <f>(I40/$Q40)*100</f>
         <v>1.7206241774769693</v>
       </c>
       <c r="T40">
-        <f t="shared" si="2"/>
+        <f>(J40/$Q40)*100</f>
         <v>0.13912389546907314</v>
       </c>
       <c r="U40">
-        <f t="shared" si="2"/>
+        <f>(K40/$Q40)*100</f>
         <v>0.71366798270351572</v>
       </c>
       <c r="V40">
-        <f t="shared" si="2"/>
+        <f>(L40/$Q40)*100</f>
         <v>0.89415303628501608</v>
       </c>
       <c r="W40">
-        <f t="shared" si="2"/>
+        <f>(M40/$Q40)*100</f>
         <v>89.5093062605753</v>
       </c>
       <c r="X40">
-        <f t="shared" si="3"/>
+        <f>(N40/$Q40)*100</f>
         <v>89.416055649558189</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="3"/>
+        <f>(O40/$Q40)*100</f>
         <v>9.3250611017108478E-2</v>
       </c>
       <c r="Z40">
-        <f t="shared" si="3"/>
+        <f>(P40/$Q40)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -4307,43 +4307,43 @@
         <v>1985.38</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="1"/>
+        <f>SUM(H41,I41,J41,K41,L41,M41,P41)</f>
         <v>2099.34</v>
       </c>
       <c r="R41">
-        <f t="shared" si="2"/>
+        <f>(H41/$Q41)*100</f>
         <v>1.3861499328360343</v>
       </c>
       <c r="S41">
-        <f t="shared" si="2"/>
+        <f>(I41/$Q41)*100</f>
         <v>0.18481999104480454</v>
       </c>
       <c r="T41">
-        <f t="shared" si="2"/>
+        <f>(J41/$Q41)*100</f>
         <v>4.7634018310516633E-2</v>
       </c>
       <c r="U41">
-        <f t="shared" si="2"/>
+        <f>(K41/$Q41)*100</f>
         <v>4.8110358493621802E-2</v>
       </c>
       <c r="V41">
-        <f t="shared" si="2"/>
+        <f>(L41/$Q41)*100</f>
         <v>0</v>
       </c>
       <c r="W41">
-        <f t="shared" si="2"/>
+        <f>(M41/$Q41)*100</f>
         <v>3.7616584259814982</v>
       </c>
       <c r="X41">
-        <f t="shared" si="3"/>
+        <f>(N41/$Q41)*100</f>
         <v>3.6559109053321519</v>
       </c>
       <c r="Y41">
-        <f t="shared" si="3"/>
+        <f>(O41/$Q41)*100</f>
         <v>0.10574752064934695</v>
       </c>
       <c r="Z41">
-        <f t="shared" si="3"/>
+        <f>(P41/$Q41)*100</f>
         <v>94.571627273333519</v>
       </c>
     </row>
@@ -4397,43 +4397,43 @@
         <v>0</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="1"/>
+        <f>SUM(H42,I42,J42,K42,L42,M42,P42)</f>
         <v>91.71</v>
       </c>
       <c r="R42">
-        <f t="shared" si="2"/>
+        <f>(H42/$Q42)*100</f>
         <v>74.572020499400296</v>
       </c>
       <c r="S42">
-        <f t="shared" si="2"/>
+        <f>(I42/$Q42)*100</f>
         <v>0.18536691745720207</v>
       </c>
       <c r="T42">
-        <f t="shared" si="2"/>
+        <f>(J42/$Q42)*100</f>
         <v>0</v>
       </c>
       <c r="U42">
-        <f t="shared" si="2"/>
+        <f>(K42/$Q42)*100</f>
         <v>7.6327554247083221E-2</v>
       </c>
       <c r="V42">
-        <f t="shared" si="2"/>
+        <f>(L42/$Q42)*100</f>
         <v>0</v>
       </c>
       <c r="W42">
-        <f t="shared" si="2"/>
+        <f>(M42/$Q42)*100</f>
         <v>25.16628502889543</v>
       </c>
       <c r="X42">
-        <f t="shared" si="3"/>
+        <f>(N42/$Q42)*100</f>
         <v>24.097699269436269</v>
       </c>
       <c r="Y42">
-        <f t="shared" si="3"/>
+        <f>(O42/$Q42)*100</f>
         <v>1.0685857594591648</v>
       </c>
       <c r="Z42">
-        <f t="shared" si="3"/>
+        <f>(P42/$Q42)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -4487,43 +4487,43 @@
         <v>0</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="1"/>
+        <f>SUM(H43,I43,J43,K43,L43,M43,P43)</f>
         <v>120.02</v>
       </c>
       <c r="R43">
-        <f t="shared" si="2"/>
+        <f>(H43/$Q43)*100</f>
         <v>41.609731711381436</v>
       </c>
       <c r="S43">
-        <f t="shared" si="2"/>
+        <f>(I43/$Q43)*100</f>
         <v>5.299116813864357</v>
       </c>
       <c r="T43">
-        <f t="shared" si="2"/>
+        <f>(J43/$Q43)*100</f>
         <v>5.740709881686386</v>
       </c>
       <c r="U43">
-        <f t="shared" si="2"/>
+        <f>(K43/$Q43)*100</f>
         <v>0.73321113147808703</v>
       </c>
       <c r="V43">
-        <f t="shared" si="2"/>
+        <f>(L43/$Q43)*100</f>
         <v>0</v>
       </c>
       <c r="W43">
-        <f t="shared" si="2"/>
+        <f>(M43/$Q43)*100</f>
         <v>46.617230461589735</v>
       </c>
       <c r="X43">
-        <f t="shared" si="3"/>
+        <f>(N43/$Q43)*100</f>
         <v>44.117647058823536</v>
       </c>
       <c r="Y43">
-        <f t="shared" si="3"/>
+        <f>(O43/$Q43)*100</f>
         <v>2.4995834027662056</v>
       </c>
       <c r="Z43">
-        <f t="shared" si="3"/>
+        <f>(P43/$Q43)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -4577,43 +4577,43 @@
         <v>0.25</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="1"/>
+        <f>SUM(H44,I44,J44,K44,L44,M44,P44)</f>
         <v>215.74</v>
       </c>
       <c r="R44">
-        <f t="shared" si="2"/>
+        <f>(H44/$Q44)*100</f>
         <v>90.196532863632157</v>
       </c>
       <c r="S44">
-        <f t="shared" si="2"/>
+        <f>(I44/$Q44)*100</f>
         <v>5.7847408918142209</v>
       </c>
       <c r="T44">
-        <f t="shared" si="2"/>
+        <f>(J44/$Q44)*100</f>
         <v>0</v>
       </c>
       <c r="U44">
-        <f t="shared" si="2"/>
+        <f>(K44/$Q44)*100</f>
         <v>0.12515064429405767</v>
       </c>
       <c r="V44">
-        <f t="shared" si="2"/>
+        <f>(L44/$Q44)*100</f>
         <v>2.3176045239640307E-2</v>
       </c>
       <c r="W44">
-        <f t="shared" si="2"/>
+        <f>(M44/$Q44)*100</f>
         <v>3.7545193288217296</v>
       </c>
       <c r="X44">
-        <f t="shared" si="3"/>
+        <f>(N44/$Q44)*100</f>
         <v>2.6652452025586353</v>
       </c>
       <c r="Y44">
-        <f t="shared" si="3"/>
+        <f>(O44/$Q44)*100</f>
         <v>1.0892741262630945</v>
       </c>
       <c r="Z44">
-        <f t="shared" si="3"/>
+        <f>(P44/$Q44)*100</f>
         <v>0.11588022619820153</v>
       </c>
     </row>
@@ -4667,43 +4667,43 @@
         <v>0</v>
       </c>
       <c r="Q45">
-        <f t="shared" si="1"/>
+        <f>SUM(H45,I45,J45,K45,L45,M45,P45)</f>
         <v>57.26</v>
       </c>
       <c r="R45">
-        <f t="shared" si="2"/>
+        <f>(H45/$Q45)*100</f>
         <v>32.221446035626968</v>
       </c>
       <c r="S45">
-        <f t="shared" si="2"/>
+        <f>(I45/$Q45)*100</f>
         <v>11.962975899406217</v>
       </c>
       <c r="T45">
-        <f t="shared" si="2"/>
+        <f>(J45/$Q45)*100</f>
         <v>0.87320991966468742</v>
       </c>
       <c r="U45">
-        <f t="shared" si="2"/>
+        <f>(K45/$Q45)*100</f>
         <v>0.209570380719525</v>
       </c>
       <c r="V45">
-        <f t="shared" si="2"/>
+        <f>(L45/$Q45)*100</f>
         <v>0</v>
       </c>
       <c r="W45">
-        <f t="shared" si="2"/>
+        <f>(M45/$Q45)*100</f>
         <v>54.732797764582607</v>
       </c>
       <c r="X45">
-        <f t="shared" si="3"/>
+        <f>(N45/$Q45)*100</f>
         <v>53.964373035277681</v>
       </c>
       <c r="Y45">
-        <f t="shared" si="3"/>
+        <f>(O45/$Q45)*100</f>
         <v>0.768424729304925</v>
       </c>
       <c r="Z45">
-        <f t="shared" si="3"/>
+        <f>(P45/$Q45)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -4757,43 +4757,43 @@
         <v>1.06</v>
       </c>
       <c r="Q46">
-        <f t="shared" si="1"/>
+        <f>SUM(H46,I46,J46,K46,L46,M46,P46)</f>
         <v>243.22</v>
       </c>
       <c r="R46">
-        <f t="shared" si="2"/>
+        <f>(H46/$Q46)*100</f>
         <v>13.761203848367732</v>
       </c>
       <c r="S46">
-        <f t="shared" si="2"/>
+        <f>(I46/$Q46)*100</f>
         <v>6.2330400460488447</v>
       </c>
       <c r="T46">
-        <f t="shared" si="2"/>
+        <f>(J46/$Q46)*100</f>
         <v>0.36592385494613933</v>
       </c>
       <c r="U46">
-        <f t="shared" si="2"/>
+        <f>(K46/$Q46)*100</f>
         <v>0.25491324726584985</v>
       </c>
       <c r="V46">
-        <f t="shared" si="2"/>
+        <f>(L46/$Q46)*100</f>
         <v>12.766219883233287</v>
       </c>
       <c r="W46">
-        <f t="shared" si="2"/>
+        <f>(M46/$Q46)*100</f>
         <v>66.182879697393304</v>
       </c>
       <c r="X46">
-        <f t="shared" si="3"/>
+        <f>(N46/$Q46)*100</f>
         <v>65.993750513937997</v>
       </c>
       <c r="Y46">
-        <f t="shared" si="3"/>
+        <f>(O46/$Q46)*100</f>
         <v>0.18912918345530796</v>
       </c>
       <c r="Z46">
-        <f t="shared" si="3"/>
+        <f>(P46/$Q46)*100</f>
         <v>0.43581942274484003</v>
       </c>
     </row>
@@ -4847,43 +4847,43 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="1"/>
+        <f>SUM(H47,I47,J47,K47,L47,M47,P47)</f>
         <v>24.33</v>
       </c>
       <c r="R47">
-        <f t="shared" si="2"/>
+        <f>(H47/$Q47)*100</f>
         <v>1.5207562679819155</v>
       </c>
       <c r="S47">
-        <f t="shared" si="2"/>
+        <f>(I47/$Q47)*100</f>
         <v>1.8495684340320593</v>
       </c>
       <c r="T47">
-        <f t="shared" si="2"/>
+        <f>(J47/$Q47)*100</f>
         <v>0</v>
       </c>
       <c r="U47">
-        <f t="shared" si="2"/>
+        <f>(K47/$Q47)*100</f>
         <v>0.61652281134401976</v>
       </c>
       <c r="V47">
-        <f t="shared" si="2"/>
+        <f>(L47/$Q47)*100</f>
         <v>0</v>
       </c>
       <c r="W47">
-        <f t="shared" si="2"/>
+        <f>(M47/$Q47)*100</f>
         <v>96.013152486641999</v>
       </c>
       <c r="X47">
-        <f t="shared" si="3"/>
+        <f>(N47/$Q47)*100</f>
         <v>96.013152486641999</v>
       </c>
       <c r="Y47">
-        <f t="shared" si="3"/>
+        <f>(O47/$Q47)*100</f>
         <v>0</v>
       </c>
       <c r="Z47">
-        <f t="shared" si="3"/>
+        <f>(P47/$Q47)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -4937,43 +4937,43 @@
         <v>0</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="1"/>
+        <f>SUM(H48,I48,J48,K48,L48,M48,P48)</f>
         <v>228.58999999999997</v>
       </c>
       <c r="R48">
-        <f t="shared" si="2"/>
+        <f>(H48/$Q48)*100</f>
         <v>2.0167111422196951</v>
       </c>
       <c r="S48">
-        <f t="shared" si="2"/>
+        <f>(I48/$Q48)*100</f>
         <v>1.0017936042696531</v>
       </c>
       <c r="T48">
-        <f t="shared" si="2"/>
+        <f>(J48/$Q48)*100</f>
         <v>0.15748720416466161</v>
       </c>
       <c r="U48">
-        <f t="shared" si="2"/>
+        <f>(K48/$Q48)*100</f>
         <v>0.39371801041165411</v>
       </c>
       <c r="V48">
-        <f t="shared" si="2"/>
+        <f>(L48/$Q48)*100</f>
         <v>8.2899514414453819</v>
       </c>
       <c r="W48">
-        <f t="shared" ref="W48:W59" si="4">(M48/$Q48)*100</f>
+        <f>(M48/$Q48)*100</f>
         <v>88.140338597488949</v>
       </c>
       <c r="X48">
-        <f t="shared" si="3"/>
+        <f>(N48/$Q48)*100</f>
         <v>88.004724616124946</v>
       </c>
       <c r="Y48">
-        <f t="shared" si="3"/>
+        <f>(O48/$Q48)*100</f>
         <v>0.1356139813640142</v>
       </c>
       <c r="Z48">
-        <f t="shared" si="3"/>
+        <f>(P48/$Q48)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -5027,43 +5027,43 @@
         <v>0</v>
       </c>
       <c r="Q49">
-        <f t="shared" si="1"/>
+        <f>SUM(H49,I49,J49,K49,L49,M49,P49)</f>
         <v>455.02</v>
       </c>
       <c r="R49">
-        <f t="shared" si="2"/>
+        <f>(H49/$Q49)*100</f>
         <v>11.46762779658037</v>
       </c>
       <c r="S49">
-        <f t="shared" si="2"/>
+        <f>(I49/$Q49)*100</f>
         <v>1.336205001977935</v>
       </c>
       <c r="T49">
-        <f t="shared" si="2"/>
+        <f>(J49/$Q49)*100</f>
         <v>2.197705595358446E-2</v>
       </c>
       <c r="U49">
-        <f t="shared" si="2"/>
+        <f>(K49/$Q49)*100</f>
         <v>0.25053843787086283</v>
       </c>
       <c r="V49">
-        <f t="shared" si="2"/>
+        <f>(L49/$Q49)*100</f>
         <v>0</v>
       </c>
       <c r="W49">
-        <f t="shared" si="4"/>
+        <f>(M49/$Q49)*100</f>
         <v>86.923651707617239</v>
       </c>
       <c r="X49">
-        <f t="shared" si="3"/>
+        <f>(N49/$Q49)*100</f>
         <v>86.750032965583941</v>
       </c>
       <c r="Y49">
-        <f t="shared" si="3"/>
+        <f>(O49/$Q49)*100</f>
         <v>0.17361874203331723</v>
       </c>
       <c r="Z49">
-        <f t="shared" si="3"/>
+        <f>(P49/$Q49)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -5117,43 +5117,43 @@
         <v>25.24</v>
       </c>
       <c r="Q50">
-        <f t="shared" si="1"/>
+        <f>SUM(H50,I50,J50,K50,L50,M50,P50)</f>
         <v>312.01</v>
       </c>
       <c r="R50">
-        <f t="shared" si="2"/>
+        <f>(H50/$Q50)*100</f>
         <v>12.97714816832794</v>
       </c>
       <c r="S50">
-        <f t="shared" si="2"/>
+        <f>(I50/$Q50)*100</f>
         <v>4.6472869459312207</v>
       </c>
       <c r="T50">
-        <f t="shared" si="2"/>
+        <f>(J50/$Q50)*100</f>
         <v>4.166533123938336E-2</v>
       </c>
       <c r="U50">
-        <f t="shared" si="2"/>
+        <f>(K50/$Q50)*100</f>
         <v>1.240344860741643</v>
       </c>
       <c r="V50">
-        <f t="shared" si="2"/>
+        <f>(L50/$Q50)*100</f>
         <v>5.589564437037275</v>
       </c>
       <c r="W50">
-        <f t="shared" si="4"/>
+        <f>(M50/$Q50)*100</f>
         <v>67.414505945322261</v>
       </c>
       <c r="X50">
-        <f t="shared" si="3"/>
+        <f>(N50/$Q50)*100</f>
         <v>66.969007403608856</v>
       </c>
       <c r="Y50">
-        <f t="shared" si="3"/>
+        <f>(O50/$Q50)*100</f>
         <v>0.44549854171340658</v>
       </c>
       <c r="Z50">
-        <f t="shared" si="3"/>
+        <f>(P50/$Q50)*100</f>
         <v>8.0894843114002768</v>
       </c>
     </row>
@@ -5207,43 +5207,43 @@
         <v>0.42</v>
       </c>
       <c r="Q51">
-        <f t="shared" si="1"/>
+        <f>SUM(H51,I51,J51,K51,L51,M51,P51)</f>
         <v>1147.69</v>
       </c>
       <c r="R51">
-        <f t="shared" si="2"/>
+        <f>(H51/$Q51)*100</f>
         <v>7.0123465395707907</v>
       </c>
       <c r="S51">
-        <f t="shared" si="2"/>
+        <f>(I51/$Q51)*100</f>
         <v>1.3261420766931837</v>
       </c>
       <c r="T51">
-        <f t="shared" si="2"/>
+        <f>(J51/$Q51)*100</f>
         <v>3.9209194120363514E-2</v>
       </c>
       <c r="U51">
-        <f t="shared" si="2"/>
+        <f>(K51/$Q51)*100</f>
         <v>1.4498688670285529</v>
       </c>
       <c r="V51">
-        <f t="shared" si="2"/>
+        <f>(L51/$Q51)*100</f>
         <v>2.7882093596702941E-2</v>
       </c>
       <c r="W51">
-        <f t="shared" si="4"/>
+        <f>(M51/$Q51)*100</f>
         <v>90.107955981144741</v>
       </c>
       <c r="X51">
-        <f t="shared" si="3"/>
+        <f>(N51/$Q51)*100</f>
         <v>90.053934424801113</v>
       </c>
       <c r="Y51">
-        <f t="shared" si="3"/>
+        <f>(O51/$Q51)*100</f>
         <v>5.402155634361195E-2</v>
       </c>
       <c r="Z51">
-        <f t="shared" si="3"/>
+        <f>(P51/$Q51)*100</f>
         <v>3.6595247845672606E-2</v>
       </c>
     </row>
@@ -5297,43 +5297,43 @@
         <v>0.01</v>
       </c>
       <c r="Q52">
-        <f t="shared" si="1"/>
+        <f>SUM(H52,I52,J52,K52,L52,M52,P52)</f>
         <v>658.62</v>
       </c>
       <c r="R52">
-        <f t="shared" si="2"/>
+        <f>(H52/$Q52)*100</f>
         <v>2.066441954389481</v>
       </c>
       <c r="S52">
-        <f t="shared" si="2"/>
+        <f>(I52/$Q52)*100</f>
         <v>1.3027238771977772</v>
       </c>
       <c r="T52">
-        <f t="shared" si="2"/>
+        <f>(J52/$Q52)*100</f>
         <v>3.0366523944004131E-2</v>
       </c>
       <c r="U52">
-        <f t="shared" si="2"/>
+        <f>(K52/$Q52)*100</f>
         <v>1.9738240563602686E-2</v>
       </c>
       <c r="V52">
-        <f t="shared" si="2"/>
+        <f>(L52/$Q52)*100</f>
         <v>0</v>
       </c>
       <c r="W52">
-        <f t="shared" si="4"/>
+        <f>(M52/$Q52)*100</f>
         <v>96.579211077707939</v>
       </c>
       <c r="X52">
-        <f t="shared" si="3"/>
+        <f>(N52/$Q52)*100</f>
         <v>96.562509489538741</v>
       </c>
       <c r="Y52">
-        <f t="shared" si="3"/>
+        <f>(O52/$Q52)*100</f>
         <v>1.670158816920227E-2</v>
       </c>
       <c r="Z52">
-        <f t="shared" si="3"/>
+        <f>(P52/$Q52)*100</f>
         <v>1.5183261972002064E-3</v>
       </c>
     </row>
@@ -5387,43 +5387,43 @@
         <v>0</v>
       </c>
       <c r="Q53">
-        <f t="shared" si="1"/>
+        <f>SUM(H53,I53,J53,K53,L53,M53,P53)</f>
         <v>536.41000000000008</v>
       </c>
       <c r="R53">
-        <f t="shared" si="2"/>
+        <f>(H53/$Q53)*100</f>
         <v>0.98059320296042185</v>
       </c>
       <c r="S53">
-        <f t="shared" si="2"/>
+        <f>(I53/$Q53)*100</f>
         <v>0.33369996830782417</v>
       </c>
       <c r="T53">
-        <f t="shared" si="2"/>
+        <f>(J53/$Q53)*100</f>
         <v>5.5927368990138136E-2</v>
       </c>
       <c r="U53">
-        <f t="shared" si="2"/>
+        <f>(K53/$Q53)*100</f>
         <v>0.2442161779236032</v>
       </c>
       <c r="V53">
-        <f t="shared" si="2"/>
+        <f>(L53/$Q53)*100</f>
         <v>48.175835648104993</v>
       </c>
       <c r="W53">
-        <f t="shared" si="4"/>
+        <f>(M53/$Q53)*100</f>
         <v>50.209727633713008</v>
       </c>
       <c r="X53">
-        <f t="shared" si="3"/>
+        <f>(N53/$Q53)*100</f>
         <v>50.17617121231892</v>
       </c>
       <c r="Y53">
-        <f t="shared" si="3"/>
+        <f>(O53/$Q53)*100</f>
         <v>3.3556421394082873E-2</v>
       </c>
       <c r="Z53">
-        <f t="shared" si="3"/>
+        <f>(P53/$Q53)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -5477,43 +5477,43 @@
         <v>0</v>
       </c>
       <c r="Q54">
-        <f t="shared" si="1"/>
+        <f>SUM(H54,I54,J54,K54,L54,M54,P54)</f>
         <v>21.93</v>
       </c>
       <c r="R54">
-        <f t="shared" si="2"/>
+        <f>(H54/$Q54)*100</f>
         <v>4.5143638850889189</v>
       </c>
       <c r="S54">
-        <f t="shared" si="2"/>
+        <f>(I54/$Q54)*100</f>
         <v>2.2799817601459189</v>
       </c>
       <c r="T54">
-        <f t="shared" si="2"/>
+        <f>(J54/$Q54)*100</f>
         <v>9.1199270405836752E-2</v>
       </c>
       <c r="U54">
-        <f t="shared" si="2"/>
+        <f>(K54/$Q54)*100</f>
         <v>0.36479708162334701</v>
       </c>
       <c r="V54">
-        <f t="shared" si="2"/>
+        <f>(L54/$Q54)*100</f>
         <v>43.866849065207475</v>
       </c>
       <c r="W54">
-        <f t="shared" si="4"/>
+        <f>(M54/$Q54)*100</f>
         <v>48.882808937528502</v>
       </c>
       <c r="X54">
-        <f t="shared" si="3"/>
+        <f>(N54/$Q54)*100</f>
         <v>48.746010031919745</v>
       </c>
       <c r="Y54">
-        <f t="shared" si="3"/>
+        <f>(O54/$Q54)*100</f>
         <v>0.13679890560875513</v>
       </c>
       <c r="Z54">
-        <f t="shared" si="3"/>
+        <f>(P54/$Q54)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -5571,39 +5571,39 @@
         <v>1525.16</v>
       </c>
       <c r="R55">
-        <f t="shared" si="2"/>
+        <f>(H55/$Q55)*100</f>
         <v>4.6113194681213772</v>
       </c>
       <c r="S55">
-        <f t="shared" si="2"/>
+        <f>(I55/$Q55)*100</f>
         <v>1.0477589236539118</v>
       </c>
       <c r="T55">
-        <f t="shared" si="2"/>
+        <f>(J55/$Q55)*100</f>
         <v>8.3269952005035536E-2</v>
       </c>
       <c r="U55">
-        <f t="shared" si="2"/>
+        <f>(K55/$Q55)*100</f>
         <v>2.7190589839754518</v>
       </c>
       <c r="V55">
-        <f t="shared" si="2"/>
+        <f>(L55/$Q55)*100</f>
         <v>1.3113378268509533E-3</v>
       </c>
       <c r="W55">
-        <f t="shared" si="4"/>
+        <f>(M55/$Q55)*100</f>
         <v>91.528757638542828</v>
       </c>
       <c r="X55">
-        <f t="shared" si="3"/>
+        <f>(N55/$Q55)*100</f>
         <v>91.461879409373438</v>
       </c>
       <c r="Y55">
-        <f t="shared" si="3"/>
+        <f>(O55/$Q55)*100</f>
         <v>6.6878229169398618E-2</v>
       </c>
       <c r="Z55">
-        <f t="shared" si="3"/>
+        <f>(P55/$Q55)*100</f>
         <v>8.523695874531197E-3</v>
       </c>
     </row>
@@ -5657,43 +5657,43 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="Q56">
-        <f t="shared" si="1"/>
+        <f>SUM(H56,I56,J56,K56,L56,M56,P56)</f>
         <v>26.589999999999996</v>
       </c>
       <c r="R56">
-        <f t="shared" si="2"/>
+        <f>(H56/$Q56)*100</f>
         <v>20.571643474990601</v>
       </c>
       <c r="S56">
-        <f t="shared" si="2"/>
+        <f>(I56/$Q56)*100</f>
         <v>5.7540428732606248</v>
       </c>
       <c r="T56">
-        <f t="shared" si="2"/>
+        <f>(J56/$Q56)*100</f>
         <v>0</v>
       </c>
       <c r="U56">
-        <f t="shared" si="2"/>
+        <f>(K56/$Q56)*100</f>
         <v>0.63933809702895839</v>
       </c>
       <c r="V56">
-        <f t="shared" si="2"/>
+        <f>(L56/$Q56)*100</f>
         <v>60.925159834524266</v>
       </c>
       <c r="W56">
-        <f t="shared" si="4"/>
+        <f>(M56/$Q56)*100</f>
         <v>11.846558856713052</v>
       </c>
       <c r="X56">
-        <f t="shared" si="3"/>
+        <f>(N56/$Q56)*100</f>
         <v>10.4550582925912</v>
       </c>
       <c r="Y56">
-        <f t="shared" si="3"/>
+        <f>(O56/$Q56)*100</f>
         <v>1.3915005641218505</v>
       </c>
       <c r="Z56">
-        <f t="shared" si="3"/>
+        <f>(P56/$Q56)*100</f>
         <v>0.26325686348251226</v>
       </c>
     </row>
@@ -5747,43 +5747,43 @@
         <v>61.85</v>
       </c>
       <c r="Q57">
-        <f t="shared" si="1"/>
+        <f>SUM(H57,I57,J57,K57,L57,M57,P57)</f>
         <v>311.22000000000003</v>
       </c>
       <c r="R57">
-        <f t="shared" si="2"/>
+        <f>(H57/$Q57)*100</f>
         <v>41.777520724889143</v>
       </c>
       <c r="S57">
-        <f t="shared" si="2"/>
+        <f>(I57/$Q57)*100</f>
         <v>3.280637491163807</v>
       </c>
       <c r="T57">
-        <f t="shared" si="2"/>
+        <f>(J57/$Q57)*100</f>
         <v>3.4862798020692756</v>
       </c>
       <c r="U57">
-        <f t="shared" si="2"/>
+        <f>(K57/$Q57)*100</f>
         <v>4.4984255510571301E-2</v>
       </c>
       <c r="V57">
-        <f t="shared" si="2"/>
+        <f>(L57/$Q57)*100</f>
         <v>4.1899620846989265</v>
       </c>
       <c r="W57">
-        <f t="shared" si="4"/>
+        <f>(M57/$Q57)*100</f>
         <v>27.347214189319452</v>
       </c>
       <c r="X57">
-        <f t="shared" si="3"/>
+        <f>(N57/$Q57)*100</f>
         <v>25.695649379859901</v>
       </c>
       <c r="Y57">
-        <f t="shared" si="3"/>
+        <f>(O57/$Q57)*100</f>
         <v>1.6515648094595461</v>
       </c>
       <c r="Z57">
-        <f t="shared" si="3"/>
+        <f>(P57/$Q57)*100</f>
         <v>19.873401452348819</v>
       </c>
     </row>
@@ -5837,43 +5837,43 @@
         <v>0</v>
       </c>
       <c r="Q58">
-        <f t="shared" si="1"/>
+        <f>SUM(H58,I58,J58,K58,L58,M58,P58)</f>
         <v>600.7399999999999</v>
       </c>
       <c r="R58">
-        <f t="shared" si="2"/>
+        <f>(H58/$Q58)*100</f>
         <v>4.4794753137796723</v>
       </c>
       <c r="S58">
-        <f t="shared" si="2"/>
+        <f>(I58/$Q58)*100</f>
         <v>0.13150447781070015</v>
       </c>
       <c r="T58">
-        <f t="shared" si="2"/>
+        <f>(J58/$Q58)*100</f>
         <v>0.14648600059926092</v>
       </c>
       <c r="U58">
-        <f t="shared" si="2"/>
+        <f>(K58/$Q58)*100</f>
         <v>7.990145487232414E-2</v>
       </c>
       <c r="V58">
-        <f t="shared" si="2"/>
+        <f>(L58/$Q58)*100</f>
         <v>0</v>
       </c>
       <c r="W58">
-        <f t="shared" si="4"/>
+        <f>(M58/$Q58)*100</f>
         <v>95.162632752938052</v>
       </c>
       <c r="X58">
-        <f t="shared" si="3"/>
+        <f>(N58/$Q58)*100</f>
         <v>95.089389752638425</v>
       </c>
       <c r="Y58">
-        <f t="shared" si="3"/>
+        <f>(O58/$Q58)*100</f>
         <v>7.3243000299630462E-2</v>
       </c>
       <c r="Z58">
-        <f t="shared" si="3"/>
+        <f>(P58/$Q58)*100</f>
         <v>0</v>
       </c>
     </row>
@@ -5902,51 +5902,75 @@
       <c r="H59" s="2">
         <v>8.9499999999999993</v>
       </c>
+      <c r="I59">
+        <v>1.22</v>
+      </c>
+      <c r="J59">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K59">
+        <v>0.38</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>314.62</v>
+      </c>
+      <c r="N59">
+        <v>314.19</v>
+      </c>
+      <c r="O59">
+        <v>0.43</v>
+      </c>
       <c r="P59">
         <v>0</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="1"/>
-        <v>8.9499999999999993</v>
+        <f>SUM(H59,I59,J59,K59,L59,M59,P59)</f>
+        <v>326.32</v>
       </c>
       <c r="R59">
-        <f t="shared" si="2"/>
-        <v>100</v>
+        <f>(H59/$Q59)*100</f>
+        <v>2.7427065457219904</v>
       </c>
       <c r="S59">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(I59/$Q59)*100</f>
+        <v>0.37386614366266241</v>
       </c>
       <c r="T59">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(J59/$Q59)*100</f>
+        <v>0.35241480755087029</v>
       </c>
       <c r="U59">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>(K59/$Q59)*100</f>
+        <v>0.11645011032115715</v>
       </c>
       <c r="V59">
-        <f t="shared" si="2"/>
+        <f>(L59/$Q59)*100</f>
         <v>0</v>
       </c>
       <c r="W59">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>(M59/$Q59)*100</f>
+        <v>96.414562392743321</v>
       </c>
       <c r="X59">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(N59/$Q59)*100</f>
+        <v>96.282789899485167</v>
       </c>
       <c r="Y59">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f>(O59/$Q59)*100</f>
+        <v>0.13177249325815149</v>
       </c>
       <c r="Z59">
-        <f t="shared" si="3"/>
+        <f>(P59/$Q59)*100</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Z59">
+    <sortCondition ref="D2:D59"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>